<commit_message>
Update GUI & Add features in HomeForm
</commit_message>
<xml_diff>
--- a/YeuCau01.xlsx
+++ b/YeuCau01.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC23C48-B7E3-4AE8-BF13-21F54E0E4CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="105">
   <si>
     <t>PHÂN CÔNG</t>
   </si>
@@ -89,17 +88,294 @@
   </si>
   <si>
     <t>S: Chính nó</t>
+  </si>
+  <si>
+    <t>NHÂN SỰ</t>
+  </si>
+  <si>
+    <t>S: chính nó
+U: ngaysinh, diachi, sodt
+I, U: (Luong, phucap =&gt; null)</t>
+  </si>
+  <si>
+    <t>S: ALL
+I, U: ALL</t>
+  </si>
+  <si>
+    <t>THONGBAO</t>
+  </si>
+  <si>
+    <t>NOI DUNG</t>
+  </si>
+  <si>
+    <t>ROWLABEL</t>
+  </si>
+  <si>
+    <t>YEU CAU 3</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>level:compartment</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>TP:MB</t>
+  </si>
+  <si>
+    <t>TP:SX</t>
+  </si>
+  <si>
+    <t>TP:GC</t>
+  </si>
+  <si>
+    <t>NV:MB</t>
+  </si>
+  <si>
+    <t>NV:SX</t>
+  </si>
+  <si>
+    <t>NV:GC</t>
+  </si>
+  <si>
+    <t>TP:SX,GC</t>
+  </si>
+  <si>
+    <t>NV:SX:B</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho nhân viên làm trong lĩnh
+vực mua bán ở miền Trung</t>
+  </si>
+  <si>
+    <t>NV:MB:T</t>
+  </si>
+  <si>
+    <t>NV:GC,SX</t>
+  </si>
+  <si>
+    <t>NV:MB:B</t>
+  </si>
+  <si>
+    <t>NV:GC:B</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả nhân viên làm trong
+lĩnh vực gia công ở miền Bắc</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho nhân viên làm trong lĩnh
+vực mua bán ở miền Bắc</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho nhân viên làm trong lĩnh
+vực sản xuất ở miền Bắc</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho nhân viên làm trong lĩnh
+sản xuất và gia công ở miền Trung</t>
+  </si>
+  <si>
+    <t>NV:SX,GC:T</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả nhân viên làm trong
+lĩnh vực gia công ở miền Nam</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho nhân viên làm trong lĩnh
+vực mua bán ở miền Nam</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho nhân viên làm trong lĩnh
+vực sản xuất ở miền Nam</t>
+  </si>
+  <si>
+    <t>NV:GC:N</t>
+  </si>
+  <si>
+    <t>NV:MB:N</t>
+  </si>
+  <si>
+    <t>NV:SX:N</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả trưởng phòng phụ trách lĩnh vực gia công ở miền Bắc</t>
+  </si>
+  <si>
+    <t>TP:GC:B</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực mua bán ở miền Bắc</t>
+  </si>
+  <si>
+    <t>TP:MB:B</t>
+  </si>
+  <si>
+    <t>TP:SX:B</t>
+  </si>
+  <si>
+    <t>level:compartment:
+group</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực mua bán ở miền Trung</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực sản xuất ở miền Bắc</t>
+  </si>
+  <si>
+    <t>TP:MB,SX,GC</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>TP:MB:T</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực sản xuất ở miền Trung</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực gia công ở miền Trung</t>
+  </si>
+  <si>
+    <t>TP:SX:T</t>
+  </si>
+  <si>
+    <t>TP:GC:T</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực gia công và sản xuất ở miền Trung</t>
+  </si>
+  <si>
+    <t>TP:GC,SX:T</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực mua bán ở miền Nam</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực sản xuất ở miền Nam</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách lĩnh
+vực gia công ở miền Nam</t>
+  </si>
+  <si>
+    <t>TP:MB:N</t>
+  </si>
+  <si>
+    <t>TP:SX:N</t>
+  </si>
+  <si>
+    <t>TP:GC:N</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách tất
+cả lĩnh vực ở miền Bắc và miền Trung</t>
+  </si>
+  <si>
+    <t>TP:SX,MB,GC:B,T</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho trưởng phòng phụ trách tất
+cả lĩnh vực ở miền Nam</t>
+  </si>
+  <si>
+    <t>TP:SX,MB,GC:N</t>
+  </si>
+  <si>
+    <t>GD:SX,MB,GC:B</t>
+  </si>
+  <si>
+    <t>GD:SX,MB,GC:T</t>
+  </si>
+  <si>
+    <t>GD:MB,SX,GC:N</t>
+  </si>
+  <si>
+    <t>GD:MB,SX,GC:N,T</t>
+  </si>
+  <si>
+    <t>X b</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả nhân viên không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả trưởng phòng không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả giám đốc không phân biệt chi nhánh: cuối năm nay sẽ thưởng 2 tháng lương.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả nhân viên làm trong lĩnh vực mua bán không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả nhân viên làm trong lĩnh vực sản xuất không phân việt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả nhân viên làm trong lĩnh vực gia công không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả nhân viên làm trong lĩnh vực gia công và sản xuất không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả trưởng phòng phụ trách lĩnh vực mua bán không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả trưởng phòng phụ trách lĩnh vực sản xuất không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả trưởng phòng phụ trách lĩnh vực gia công không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả trưởng phòng phụ trách lĩnh vực sản xuất và gia công không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho tất cả trưởng phòng phụ trách tất cả lĩnh vực không phân biệt chi nhánh.</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho giám đốc phụ trách tất cả lĩnh vực ở chi nhánh miền Bắc</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho giám đốc phụ trách tất cả 
+lĩnh vực ở chi nhánh miền Nam</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho giám đốc phụ trách tất cả lĩnh vực chi nhánh miền Trung</t>
+  </si>
+  <si>
+    <t>Thông báo này dành cho giám đốc phụ trách quản
+lý tất cả lĩnh vực chi nhánh miền Nam và miền Trung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -109,8 +385,16 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -129,8 +413,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -153,11 +442,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -175,8 +495,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,20 +803,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="E40" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="7" width="20.75" customWidth="1"/>
+    <col min="3" max="7" width="20.77734375" customWidth="1"/>
+    <col min="9" max="9" width="45.77734375" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -482,7 +833,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:11" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -499,7 +850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="3:7" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:11" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
@@ -516,7 +867,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:11" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
@@ -533,14 +884,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="79.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -550,7 +901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:11" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
@@ -567,7 +918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="79.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:11" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
@@ -583,6 +934,512 @@
       <c r="G8" s="6" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="9" spans="3:11" s="8" customFormat="1" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="H15" s="10"/>
+      <c r="I15" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="3:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="10">
+        <v>1</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H17" s="10">
+        <v>2</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H18" s="10">
+        <v>3</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="10">
+        <v>4</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H20" s="10">
+        <v>5</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H21" s="10">
+        <v>6</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="7:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H22" s="10">
+        <v>7</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H23" s="10">
+        <v>8</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H24" s="10">
+        <v>9</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H25" s="10">
+        <v>10</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="7:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H26" s="10">
+        <v>11</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H27" s="10">
+        <v>12</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G28" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="10">
+        <v>13</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28" s="10"/>
+      <c r="L28" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H29" s="10">
+        <v>14</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="10"/>
+    </row>
+    <row r="30" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H30" s="10">
+        <v>15</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H31" s="10">
+        <v>16</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="7:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H32" s="10">
+        <v>17</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H33" s="10">
+        <v>18</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H34" s="10">
+        <v>19</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H35" s="10">
+        <v>20</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="10"/>
+    </row>
+    <row r="36" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H36" s="10">
+        <v>21</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K36" s="10"/>
+      <c r="L36" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H37" s="10">
+        <v>22</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K37" s="10"/>
+      <c r="L37" s="13"/>
+    </row>
+    <row r="38" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H38" s="16">
+        <v>23</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K38" s="10"/>
+      <c r="L38" s="13"/>
+    </row>
+    <row r="39" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H39" s="16">
+        <v>24</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K39" s="14"/>
+      <c r="L39" s="13"/>
+    </row>
+    <row r="40" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H40" s="16">
+        <v>25</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K40" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="L40" s="13"/>
+    </row>
+    <row r="41" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H41" s="16">
+        <v>26</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K41" s="14"/>
+    </row>
+    <row r="42" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H42" s="16">
+        <v>27</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K42" s="14"/>
+    </row>
+    <row r="43" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H43" s="16">
+        <v>28</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K43" s="14"/>
+    </row>
+    <row r="44" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H44" s="16">
+        <v>29</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="K44" s="14"/>
+    </row>
+    <row r="45" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H45" s="16">
+        <v>30</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K45" s="14"/>
+    </row>
+    <row r="46" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H46" s="16">
+        <v>31</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J46" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H47" s="16">
+        <v>32</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J47" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="8:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H48" s="16">
+        <v>33</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="J48" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="K48" s="14"/>
+      <c r="L48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="8:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H49" s="16">
+        <v>34</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="J49" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="K49" s="14"/>
+    </row>
+    <row r="50" spans="8:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H50" s="16">
+        <v>35</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J50" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="K50" s="14"/>
+    </row>
+    <row r="51" spans="8:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H51" s="16">
+        <v>36</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="J51" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="K51" s="14"/>
+    </row>
+    <row r="52" spans="8:11" x14ac:dyDescent="0.3">
+      <c r="H52" s="16"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>